<commit_message>
added scatter_plot, modified data generation
</commit_message>
<xml_diff>
--- a/data/distribution_data.xlsx
+++ b/data/distribution_data.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajad/PycharmProjects/EORScreeningAPP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajad/PycharmProjects/EORScreeningAPP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4E3E244-1900-7E49-AE2C-0CA7AC0FB09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CF7AD5-7CE9-9649-ADE4-D25488B5BB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21420" yWindow="0" windowWidth="27640" windowHeight="16440" xr2:uid="{965F3462-85CA-B643-B2A9-AA69C4853DCF}"/>
+    <workbookView xWindow="400" yWindow="760" windowWidth="27640" windowHeight="17240" activeTab="3" xr2:uid="{965F3462-85CA-B643-B2A9-AA69C4853DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="average" sheetId="1" r:id="rId1"/>
     <sheet name="std_dev" sheetId="2" r:id="rId2"/>
+    <sheet name="min" sheetId="3" r:id="rId3"/>
+    <sheet name="max" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
   <si>
     <t>Chemical</t>
   </si>
@@ -94,8 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
@@ -300,56 +301,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -394,6 +365,60 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -712,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2BDF88-9FF6-3D40-A70B-003A59E5961D}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,28 +747,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -751,51 +776,51 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="12">
         <v>2.5910000000000002</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="11">
         <v>20.2</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="11">
         <v>25.3</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="13">
         <v>1.2829999999999999</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="25">
         <v>4241</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="25">
         <v>135</v>
       </c>
-      <c r="H2" s="21">
+      <c r="H2" s="25">
         <v>57.4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="15">
         <v>2.3531047206266873</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="14">
         <v>25.9</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="14">
         <v>22.3</v>
       </c>
-      <c r="E3" s="26">
+      <c r="E3" s="16">
         <v>1.4246243019682843</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="19">
         <v>3805.8</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="19">
         <v>131.69999999999999</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="19">
         <v>51.9</v>
       </c>
     </row>
@@ -803,155 +828,155 @@
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="12">
         <v>1.3377668542152081</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="11">
         <v>14.7</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="11">
         <v>36.9</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="13">
         <v>7.9839377915459322E-2</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="25">
         <v>6110</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="25">
         <v>137.5</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="25">
         <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="15">
         <v>2.2796250080689227</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="14">
         <v>13.9</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="14">
         <v>38.200000000000003</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="16">
         <v>-0.26145855238870103</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="19">
         <v>7992</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="19">
         <v>196.7</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="19">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="12">
         <v>1.0921258487308312</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="17">
         <v>17.3</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="17">
         <v>32.1</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="13">
         <v>0.30512322433177025</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="26">
         <v>8791.7000000000007</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="26">
         <v>212.7</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <v>62.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="15">
         <v>3.1934332648096246</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="18">
         <v>27.2</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="18">
         <v>18</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="16">
         <v>2.2350252985147163</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="39">
         <v>2998</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="39">
         <v>124.2</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="39">
         <v>72.3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="12">
         <v>2.4261291493477959</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="11">
         <v>19.899999999999999</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="11">
         <v>28.3</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="13">
         <v>0.37712077025078661</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="25">
         <v>8330</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="25">
         <v>187.2</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="25">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="20">
         <v>0.65404654767698034</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="19">
         <v>11.516666666666666</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="19">
         <v>48.166666666666664</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="21">
         <v>-0.82159877970997996</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="19">
         <v>14316.666666666666</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="19">
         <v>247.33333333333334</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="19">
         <v>76.3</v>
       </c>
     </row>
@@ -959,25 +984,25 @@
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="12">
         <v>3.1808062765568819</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="11">
         <v>32</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="11">
         <v>14.3</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="13">
         <v>3.2218506036203021</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="25">
         <v>1612</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="25">
         <v>106.3</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="25">
         <v>65.400000000000006</v>
       </c>
     </row>
@@ -990,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDFE6D8-BA75-984C-886D-6F70ACE0962F}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B2" activeCellId="1" sqref="E2:E10 B2:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,28 +1025,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1029,51 +1054,51 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="12">
         <v>0.54473848181956452</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="25">
         <v>6.4035060667153605</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="25">
         <v>8.3319072347066552</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="12">
         <v>0.97780082615281261</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="29">
         <v>2455.1890400108041</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="25">
         <v>40.724889162077936</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="34">
         <v>13.75841293647682</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="15">
         <v>0.46737895432693638</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="19">
         <v>6.0331160181856918</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="19">
         <v>7.0445692242716689</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="15">
         <v>0.89926610210782887</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="30">
         <v>1450.0170880219155</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="19">
         <v>21.242096569469471</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="35">
         <v>14.648426157403016</v>
       </c>
     </row>
@@ -1081,155 +1106,155 @@
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="12">
         <v>0.75179083629358556</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="25">
         <v>6.1929556665234564</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="25">
         <v>4.2366999984209377</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="12">
         <v>0.30207660105675149</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="29">
         <v>1888.421263542627</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="25">
         <v>35.15786965001643</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="34">
         <v>14.337228831263015</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="15">
         <v>0.83277930927972044</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="19">
         <v>6.0787666226831831</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="19">
         <v>7.3637328835727027</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="15">
         <v>0.52219663749317025</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="30">
         <v>2685.0710061694358</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="19">
         <v>41.125782583128931</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="35">
         <v>20.309769707264781</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="22">
         <v>0.25706380643386512</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="26">
         <v>1.6562172428626494</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="26">
         <v>3.3548782889001107</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="22">
         <v>0.15505528239355609</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="31">
         <v>777.85093901938137</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="26">
         <v>8.807745959602201</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="36">
         <v>13.206690223771687</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="23">
         <v>0.63858410278212574</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="27">
         <v>5.2982078023761732</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="27">
         <v>6.0343297966447444</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="23">
         <v>0.81313380491777765</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="32">
         <v>2686.7218702880327</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="27">
         <v>45.14541396827434</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="37">
         <v>9.2843064957722081</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="24">
         <v>0.92577049812603718</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="28">
         <v>6.7704331790586858</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="28">
         <v>6.1941031296101974</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="24">
         <v>0.60937257383368992</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="33">
         <v>1228.4960191778412</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="28">
         <v>49.622525749183659</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="38">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="15">
         <v>0.69476192543911641</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="19">
         <v>2.0043009310535793</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="19">
         <v>5.6100108932356116</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="15">
         <v>0.24376529988996748</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="30">
         <v>3369.1822285072217</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="19">
         <v>65.870242817898344</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="35">
         <v>16.606023003717656</v>
       </c>
     </row>
@@ -1237,26 +1262,582 @@
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="12">
         <v>0.56005906706868247</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="25">
         <v>5.766254753091582</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="25">
         <v>4.5529650813928386</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="12">
         <v>0.85204238054843051</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="29">
         <v>888.67253538982789</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="25">
         <v>32.929128249088194</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="34">
         <v>12.367642057042737</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8FA703-6056-6C4B-91B3-0363B1D85E83}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>1.5</v>
+      </c>
+      <c r="C2" s="25">
+        <v>10</v>
+      </c>
+      <c r="D2" s="25">
+        <v>14</v>
+      </c>
+      <c r="E2" s="12">
+        <v>-0.4</v>
+      </c>
+      <c r="F2" s="25">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="25">
+        <v>60</v>
+      </c>
+      <c r="H2" s="34">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1.7</v>
+      </c>
+      <c r="C3" s="19">
+        <v>16</v>
+      </c>
+      <c r="D3" s="19">
+        <v>11</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="19">
+        <v>80</v>
+      </c>
+      <c r="H3" s="35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="C4" s="25">
+        <v>7</v>
+      </c>
+      <c r="D4" s="25">
+        <v>30</v>
+      </c>
+      <c r="E4" s="12">
+        <v>-0.5</v>
+      </c>
+      <c r="F4" s="25">
+        <v>3000</v>
+      </c>
+      <c r="G4" s="25">
+        <v>90</v>
+      </c>
+      <c r="H4" s="34">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="19">
+        <v>4</v>
+      </c>
+      <c r="D5" s="19">
+        <v>25</v>
+      </c>
+      <c r="E5" s="15">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="19">
+        <v>3800</v>
+      </c>
+      <c r="G5" s="19">
+        <v>130</v>
+      </c>
+      <c r="H5" s="35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="C6" s="26">
+        <v>14</v>
+      </c>
+      <c r="D6" s="26">
+        <v>30</v>
+      </c>
+      <c r="E6" s="22">
+        <v>-0.3</v>
+      </c>
+      <c r="F6" s="26">
+        <v>7500</v>
+      </c>
+      <c r="G6" s="26">
+        <v>198</v>
+      </c>
+      <c r="H6" s="36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="23">
+        <v>2</v>
+      </c>
+      <c r="C7" s="27">
+        <v>18</v>
+      </c>
+      <c r="D7" s="27">
+        <v>10</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="27">
+        <v>400</v>
+      </c>
+      <c r="G7" s="27">
+        <v>65</v>
+      </c>
+      <c r="H7" s="37">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="C8" s="28">
+        <v>14</v>
+      </c>
+      <c r="D8" s="28">
+        <v>20</v>
+      </c>
+      <c r="E8" s="24">
+        <v>-0.5</v>
+      </c>
+      <c r="F8" s="28">
+        <v>6000</v>
+      </c>
+      <c r="G8" s="28">
+        <v>140</v>
+      </c>
+      <c r="H8" s="38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="15">
+        <v>0</v>
+      </c>
+      <c r="C9" s="19">
+        <v>5</v>
+      </c>
+      <c r="D9" s="19">
+        <v>38</v>
+      </c>
+      <c r="E9" s="15">
+        <v>-1.2</v>
+      </c>
+      <c r="F9" s="19">
+        <v>10000</v>
+      </c>
+      <c r="G9" s="19">
+        <v>150</v>
+      </c>
+      <c r="H9" s="35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C10" s="25">
+        <v>20</v>
+      </c>
+      <c r="D10" s="25">
+        <v>8</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="F10" s="25">
+        <v>300</v>
+      </c>
+      <c r="G10" s="25">
+        <v>50</v>
+      </c>
+      <c r="H10" s="34">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC68383D-9663-0843-9FA1-43EE6A2D335A}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12">
+        <v>3.7</v>
+      </c>
+      <c r="C2" s="25">
+        <v>35</v>
+      </c>
+      <c r="D2" s="25">
+        <v>40</v>
+      </c>
+      <c r="E2" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F2" s="25">
+        <v>7000</v>
+      </c>
+      <c r="G2" s="25">
+        <v>200</v>
+      </c>
+      <c r="H2" s="34">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="15">
+        <v>3.1</v>
+      </c>
+      <c r="C3" s="19">
+        <v>33</v>
+      </c>
+      <c r="D3" s="19">
+        <v>33</v>
+      </c>
+      <c r="E3" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="F3" s="19">
+        <v>6000</v>
+      </c>
+      <c r="G3" s="19">
+        <v>180</v>
+      </c>
+      <c r="H3" s="35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2.6</v>
+      </c>
+      <c r="C4" s="25">
+        <v>26</v>
+      </c>
+      <c r="D4" s="25">
+        <v>44</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="25">
+        <v>9500</v>
+      </c>
+      <c r="G4" s="25">
+        <v>190</v>
+      </c>
+      <c r="H4" s="34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="15">
+        <v>3.6</v>
+      </c>
+      <c r="C5" s="19">
+        <v>26</v>
+      </c>
+      <c r="D5" s="19">
+        <v>52</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="19">
+        <v>13000</v>
+      </c>
+      <c r="G5" s="19">
+        <v>260</v>
+      </c>
+      <c r="H5" s="35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="22">
+        <v>1.7</v>
+      </c>
+      <c r="C6" s="26">
+        <v>21</v>
+      </c>
+      <c r="D6" s="26">
+        <v>35</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="26">
+        <v>10000</v>
+      </c>
+      <c r="G6" s="26">
+        <v>225</v>
+      </c>
+      <c r="H6" s="36">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="23">
+        <v>4.5</v>
+      </c>
+      <c r="C7" s="27">
+        <v>36</v>
+      </c>
+      <c r="D7" s="27">
+        <v>22</v>
+      </c>
+      <c r="E7" s="23">
+        <v>3.5</v>
+      </c>
+      <c r="F7" s="27">
+        <v>4000</v>
+      </c>
+      <c r="G7" s="27">
+        <v>185</v>
+      </c>
+      <c r="H7" s="37">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="24">
+        <v>3.5</v>
+      </c>
+      <c r="C8" s="28">
+        <v>26</v>
+      </c>
+      <c r="D8" s="28">
+        <v>40</v>
+      </c>
+      <c r="E8" s="24">
+        <v>1.3</v>
+      </c>
+      <c r="F8" s="28">
+        <v>10500</v>
+      </c>
+      <c r="G8" s="28">
+        <v>240</v>
+      </c>
+      <c r="H8" s="38">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="15">
+        <v>1.7</v>
+      </c>
+      <c r="C9" s="19">
+        <v>20</v>
+      </c>
+      <c r="D9" s="19">
+        <v>55</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0</v>
+      </c>
+      <c r="F9" s="19">
+        <v>18000</v>
+      </c>
+      <c r="G9" s="19">
+        <v>300</v>
+      </c>
+      <c r="H9" s="35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="12">
+        <v>4</v>
+      </c>
+      <c r="C10" s="25">
+        <v>40</v>
+      </c>
+      <c r="D10" s="25">
+        <v>20</v>
+      </c>
+      <c r="E10" s="12">
+        <v>4.8</v>
+      </c>
+      <c r="F10" s="25">
+        <v>3000</v>
+      </c>
+      <c r="G10" s="25">
+        <v>150</v>
+      </c>
+      <c r="H10" s="34">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test_data_401 to Excel file
</commit_message>
<xml_diff>
--- a/data/distribution_data.xlsx
+++ b/data/distribution_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sajad/PycharmProjects/EORScreeningAPP/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAA7D67-65CC-D240-8D01-D2A53380BE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30674188-5D39-4E4B-9328-76423EEAFE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34100" yWindow="-1960" windowWidth="31580" windowHeight="20680" activeTab="4" xr2:uid="{965F3462-85CA-B643-B2A9-AA69C4853DCF}"/>
+    <workbookView xWindow="-34100" yWindow="-1960" windowWidth="31580" windowHeight="20680" activeTab="5" xr2:uid="{965F3462-85CA-B643-B2A9-AA69C4853DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="average" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,6 @@
     <sheet name="test_data_364" sheetId="5" r:id="rId5"/>
     <sheet name="test_data_401" sheetId="6" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <definedNames>
     <definedName name="table_4" localSheetId="5">#REF!</definedName>
     <definedName name="table_4">#REF!</definedName>
@@ -1649,34 +1646,34 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1703,40 +1700,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Selected Data"/>
-      <sheetName val="Averages-MinMax"/>
-      <sheetName val="Averages-MinMax (2)"/>
-      <sheetName val="Data-(548)"/>
-      <sheetName val="Data-(536)-nomicrobia"/>
-      <sheetName val="Data-(536)-Fields Tab"/>
-      <sheetName val="Data-Validation(401)"/>
-      <sheetName val="Data - Validation - EORgui"/>
-      <sheetName val="PCA variances"/>
-      <sheetName val="Database - 3 - new database"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3150,7 +3113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DB51D2-E446-8D47-9E87-E87789F11451}">
   <dimension ref="A1:H365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A335" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="I356" sqref="I356"/>
     </sheetView>
   </sheetViews>
@@ -12658,8 +12621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C687BEC1-2946-BA45-B307-F386C4DE0079}">
   <dimension ref="A1:P537"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P80" sqref="P80"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12682,7 +12645,7 @@
     <col min="16" max="16384" width="10.6640625" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="53" t="s">
         <v>17</v>
       </c>

</xml_diff>